<commit_message>
Updated error handling to send email on error and on failed login
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6f5c3159d118c67/Documents/UiPath/Calculate Client Security Hash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C2ACEA-E29F-4DDE-B49D-5F80DC5B82FA}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E9ADF41-E123-4BE6-9802-888E621DC4B0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1633,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>